<commit_message>
Excel to pdf functionality added
</commit_message>
<xml_diff>
--- a/templates/Submission Summary-Kramerica Inc-2025-04-28T22_19_05.8370782Z.xlsx
+++ b/templates/Submission Summary-Kramerica Inc-2025-04-28T22_19_05.8370782Z.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC25CC76-4D19-4856-BB92-A95492F64DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F003E86-94E0-4650-B791-9A5BA60CCC8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Template (2)" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Summary Template (2)'!$A$1:$AQ$35</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
@@ -26,9 +29,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="85">
-  <si>
-    <t>{{INSURED FEIN}}</t>
-  </si>
   <si>
     <t>Submission Summary</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>Total Claim Count  Reported</t>
+  </si>
+  <si>
+    <t>{{placeholder}}</t>
   </si>
 </sst>
 </file>
@@ -1063,84 +1066,98 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1158,80 +1175,66 @@
     <xf numFmtId="166" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1592,8 +1595,8 @@
   </sheetPr>
   <dimension ref="A1:BI1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" zoomScale="41" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BK20" sqref="BK20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1777,9 +1780,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="L3" s="3"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -1837,7 +1838,7 @@
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -1845,14 +1846,14 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="6"/>
+      <c r="L4" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="101" t="s">
-        <v>3</v>
-      </c>
-      <c r="M4" s="102"/>
-      <c r="N4" s="103"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="90"/>
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6">
@@ -1860,31 +1861,31 @@
       </c>
       <c r="R4" s="6"/>
       <c r="S4" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
       <c r="X4" s="6"/>
-      <c r="Y4" s="104" t="s">
-        <v>5</v>
+      <c r="Y4" s="91" t="s">
+        <v>4</v>
       </c>
-      <c r="Z4" s="102"/>
-      <c r="AA4" s="102"/>
-      <c r="AB4" s="102"/>
-      <c r="AC4" s="102"/>
-      <c r="AD4" s="102"/>
-      <c r="AE4" s="102"/>
-      <c r="AF4" s="102"/>
-      <c r="AG4" s="102"/>
-      <c r="AH4" s="102"/>
-      <c r="AI4" s="102"/>
-      <c r="AJ4" s="102"/>
-      <c r="AK4" s="102"/>
-      <c r="AL4" s="102"/>
-      <c r="AM4" s="102"/>
-      <c r="AN4" s="103"/>
+      <c r="Z4" s="89"/>
+      <c r="AA4" s="89"/>
+      <c r="AB4" s="89"/>
+      <c r="AC4" s="89"/>
+      <c r="AD4" s="89"/>
+      <c r="AE4" s="89"/>
+      <c r="AF4" s="89"/>
+      <c r="AG4" s="89"/>
+      <c r="AH4" s="89"/>
+      <c r="AI4" s="89"/>
+      <c r="AJ4" s="89"/>
+      <c r="AK4" s="89"/>
+      <c r="AL4" s="89"/>
+      <c r="AM4" s="89"/>
+      <c r="AN4" s="90"/>
       <c r="AO4" s="8"/>
       <c r="AP4" s="9"/>
       <c r="AQ4" s="1"/>
@@ -1913,48 +1914,48 @@
         <v>1.2</v>
       </c>
       <c r="C5" s="11"/>
-      <c r="D5" s="105" t="s">
+      <c r="D5" s="92" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="57"/>
-      <c r="K5" s="107" t="s">
-        <v>7</v>
-      </c>
-      <c r="L5" s="108"/>
-      <c r="M5" s="108"/>
-      <c r="N5" s="108"/>
-      <c r="O5" s="108"/>
-      <c r="P5" s="108"/>
-      <c r="Q5" s="108"/>
-      <c r="R5" s="108"/>
-      <c r="S5" s="108"/>
-      <c r="T5" s="108"/>
-      <c r="U5" s="108"/>
-      <c r="V5" s="108"/>
-      <c r="W5" s="108"/>
-      <c r="X5" s="108"/>
-      <c r="Y5" s="108"/>
-      <c r="Z5" s="108"/>
-      <c r="AA5" s="108"/>
-      <c r="AB5" s="108"/>
-      <c r="AC5" s="108"/>
-      <c r="AD5" s="108"/>
-      <c r="AE5" s="108"/>
-      <c r="AF5" s="108"/>
-      <c r="AG5" s="108"/>
-      <c r="AH5" s="108"/>
-      <c r="AI5" s="108"/>
-      <c r="AJ5" s="108"/>
-      <c r="AK5" s="108"/>
-      <c r="AL5" s="108"/>
-      <c r="AM5" s="108"/>
-      <c r="AN5" s="108"/>
-      <c r="AO5" s="109"/>
+      <c r="L5" s="94"/>
+      <c r="M5" s="94"/>
+      <c r="N5" s="94"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="94"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="94"/>
+      <c r="S5" s="94"/>
+      <c r="T5" s="94"/>
+      <c r="U5" s="94"/>
+      <c r="V5" s="94"/>
+      <c r="W5" s="94"/>
+      <c r="X5" s="94"/>
+      <c r="Y5" s="94"/>
+      <c r="Z5" s="94"/>
+      <c r="AA5" s="94"/>
+      <c r="AB5" s="94"/>
+      <c r="AC5" s="94"/>
+      <c r="AD5" s="94"/>
+      <c r="AE5" s="94"/>
+      <c r="AF5" s="94"/>
+      <c r="AG5" s="94"/>
+      <c r="AH5" s="94"/>
+      <c r="AI5" s="94"/>
+      <c r="AJ5" s="94"/>
+      <c r="AK5" s="94"/>
+      <c r="AL5" s="94"/>
+      <c r="AM5" s="94"/>
+      <c r="AN5" s="94"/>
+      <c r="AO5" s="95"/>
       <c r="AP5" s="9"/>
       <c r="AQ5" s="1"/>
       <c r="AR5" s="1"/>
@@ -1982,44 +1983,46 @@
         <v>1.3</v>
       </c>
       <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="D6" s="13" t="s">
+        <v>84</v>
+      </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
-      <c r="H6" s="113"/>
-      <c r="I6" s="114"/>
-      <c r="J6" s="115"/>
-      <c r="K6" s="110"/>
-      <c r="L6" s="111"/>
-      <c r="M6" s="111"/>
-      <c r="N6" s="111"/>
-      <c r="O6" s="111"/>
-      <c r="P6" s="111"/>
-      <c r="Q6" s="111"/>
-      <c r="R6" s="111"/>
-      <c r="S6" s="111"/>
-      <c r="T6" s="111"/>
-      <c r="U6" s="111"/>
-      <c r="V6" s="111"/>
-      <c r="W6" s="111"/>
-      <c r="X6" s="111"/>
-      <c r="Y6" s="111"/>
-      <c r="Z6" s="111"/>
-      <c r="AA6" s="111"/>
-      <c r="AB6" s="111"/>
-      <c r="AC6" s="111"/>
-      <c r="AD6" s="111"/>
-      <c r="AE6" s="111"/>
-      <c r="AF6" s="111"/>
-      <c r="AG6" s="111"/>
-      <c r="AH6" s="111"/>
-      <c r="AI6" s="111"/>
-      <c r="AJ6" s="111"/>
-      <c r="AK6" s="111"/>
-      <c r="AL6" s="111"/>
-      <c r="AM6" s="111"/>
-      <c r="AN6" s="111"/>
-      <c r="AO6" s="112"/>
+      <c r="H6" s="98"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="96"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="69"/>
+      <c r="N6" s="69"/>
+      <c r="O6" s="69"/>
+      <c r="P6" s="69"/>
+      <c r="Q6" s="69"/>
+      <c r="R6" s="69"/>
+      <c r="S6" s="69"/>
+      <c r="T6" s="69"/>
+      <c r="U6" s="69"/>
+      <c r="V6" s="69"/>
+      <c r="W6" s="69"/>
+      <c r="X6" s="69"/>
+      <c r="Y6" s="69"/>
+      <c r="Z6" s="69"/>
+      <c r="AA6" s="69"/>
+      <c r="AB6" s="69"/>
+      <c r="AC6" s="69"/>
+      <c r="AD6" s="69"/>
+      <c r="AE6" s="69"/>
+      <c r="AF6" s="69"/>
+      <c r="AG6" s="69"/>
+      <c r="AH6" s="69"/>
+      <c r="AI6" s="69"/>
+      <c r="AJ6" s="69"/>
+      <c r="AK6" s="69"/>
+      <c r="AL6" s="69"/>
+      <c r="AM6" s="69"/>
+      <c r="AN6" s="69"/>
+      <c r="AO6" s="97"/>
       <c r="AP6" s="9"/>
       <c r="AQ6" s="14"/>
       <c r="AR6" s="1"/>
@@ -2048,7 +2051,7 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -2057,11 +2060,11 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="121" t="s">
-        <v>9</v>
+      <c r="L7" s="81" t="s">
+        <v>8</v>
       </c>
-      <c r="M7" s="61"/>
-      <c r="N7" s="62"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="58"/>
       <c r="O7" s="16"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="17">
@@ -2069,7 +2072,7 @@
       </c>
       <c r="R7" s="18"/>
       <c r="S7" s="19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="T7" s="18"/>
       <c r="U7" s="18"/>
@@ -2081,22 +2084,22 @@
       <c r="AA7" s="18"/>
       <c r="AB7" s="18"/>
       <c r="AC7" s="18"/>
-      <c r="AD7" s="116" t="s">
+      <c r="AD7" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE7" s="57"/>
+      <c r="AF7" s="57"/>
+      <c r="AG7" s="58"/>
+      <c r="AH7" s="18"/>
+      <c r="AI7" s="18"/>
+      <c r="AJ7" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="AE7" s="61"/>
-      <c r="AF7" s="61"/>
-      <c r="AG7" s="62"/>
-      <c r="AH7" s="18"/>
-      <c r="AI7" s="18"/>
-      <c r="AJ7" s="116" t="s">
-        <v>12</v>
-      </c>
-      <c r="AK7" s="61"/>
-      <c r="AL7" s="61"/>
-      <c r="AM7" s="61"/>
-      <c r="AN7" s="61"/>
-      <c r="AO7" s="117"/>
+      <c r="AK7" s="57"/>
+      <c r="AL7" s="57"/>
+      <c r="AM7" s="57"/>
+      <c r="AN7" s="57"/>
+      <c r="AO7" s="79"/>
       <c r="AP7" s="9"/>
       <c r="AQ7" s="1"/>
       <c r="AR7" s="1"/>
@@ -2125,7 +2128,7 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -2134,11 +2137,11 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="122" t="s">
-        <v>14</v>
+      <c r="L8" s="56" t="s">
+        <v>13</v>
       </c>
-      <c r="M8" s="61"/>
-      <c r="N8" s="62"/>
+      <c r="M8" s="57"/>
+      <c r="N8" s="58"/>
       <c r="O8" s="16"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="20">
@@ -2146,36 +2149,36 @@
       </c>
       <c r="R8" s="1"/>
       <c r="S8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
-      <c r="Y8" s="123" t="s">
-        <v>16</v>
+      <c r="Y8" s="82" t="s">
+        <v>15</v>
       </c>
-      <c r="Z8" s="61"/>
-      <c r="AA8" s="61"/>
-      <c r="AB8" s="61"/>
-      <c r="AC8" s="62"/>
-      <c r="AD8" s="63">
+      <c r="Z8" s="57"/>
+      <c r="AA8" s="57"/>
+      <c r="AB8" s="57"/>
+      <c r="AC8" s="58"/>
+      <c r="AD8" s="80">
         <v>3</v>
       </c>
-      <c r="AE8" s="61"/>
-      <c r="AF8" s="61"/>
-      <c r="AG8" s="62"/>
+      <c r="AE8" s="57"/>
+      <c r="AF8" s="57"/>
+      <c r="AG8" s="58"/>
       <c r="AH8" s="1"/>
       <c r="AI8" s="1"/>
-      <c r="AJ8" s="63">
+      <c r="AJ8" s="80">
         <v>15</v>
       </c>
-      <c r="AK8" s="61"/>
-      <c r="AL8" s="61"/>
-      <c r="AM8" s="61"/>
-      <c r="AN8" s="61"/>
-      <c r="AO8" s="117"/>
+      <c r="AK8" s="57"/>
+      <c r="AL8" s="57"/>
+      <c r="AM8" s="57"/>
+      <c r="AN8" s="57"/>
+      <c r="AO8" s="79"/>
       <c r="AP8" s="9"/>
       <c r="AQ8" s="1"/>
       <c r="AR8" s="1"/>
@@ -2204,7 +2207,7 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -2213,11 +2216,11 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="122" t="s">
-        <v>18</v>
+      <c r="L9" s="56" t="s">
+        <v>17</v>
       </c>
-      <c r="M9" s="61"/>
-      <c r="N9" s="62"/>
+      <c r="M9" s="57"/>
+      <c r="N9" s="58"/>
       <c r="O9" s="16"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="20">
@@ -2225,36 +2228,36 @@
       </c>
       <c r="R9" s="1"/>
       <c r="S9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
-      <c r="Y9" s="124" t="s">
+      <c r="Y9" s="83" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z9" s="57"/>
+      <c r="AA9" s="57"/>
+      <c r="AB9" s="57"/>
+      <c r="AC9" s="58"/>
+      <c r="AD9" s="80">
+        <v>3</v>
+      </c>
+      <c r="AE9" s="57"/>
+      <c r="AF9" s="57"/>
+      <c r="AG9" s="58"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
+      <c r="AJ9" s="87">
         <v>20</v>
       </c>
-      <c r="Z9" s="61"/>
-      <c r="AA9" s="61"/>
-      <c r="AB9" s="61"/>
-      <c r="AC9" s="62"/>
-      <c r="AD9" s="63">
-        <v>3</v>
-      </c>
-      <c r="AE9" s="61"/>
-      <c r="AF9" s="61"/>
-      <c r="AG9" s="62"/>
-      <c r="AH9" s="1"/>
-      <c r="AI9" s="1"/>
-      <c r="AJ9" s="118">
-        <v>20</v>
-      </c>
-      <c r="AK9" s="61"/>
-      <c r="AL9" s="61"/>
-      <c r="AM9" s="61"/>
-      <c r="AN9" s="61"/>
-      <c r="AO9" s="117"/>
+      <c r="AK9" s="57"/>
+      <c r="AL9" s="57"/>
+      <c r="AM9" s="57"/>
+      <c r="AN9" s="57"/>
+      <c r="AO9" s="79"/>
       <c r="AP9" s="9"/>
       <c r="AQ9" s="1"/>
       <c r="AR9" s="1"/>
@@ -2283,7 +2286,7 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -2292,11 +2295,11 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="122" t="s">
-        <v>22</v>
+      <c r="L10" s="56" t="s">
+        <v>21</v>
       </c>
-      <c r="M10" s="61"/>
-      <c r="N10" s="62"/>
+      <c r="M10" s="57"/>
+      <c r="N10" s="58"/>
       <c r="O10" s="16"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="20">
@@ -2304,36 +2307,36 @@
       </c>
       <c r="R10" s="1"/>
       <c r="S10" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T10" s="21"/>
       <c r="U10" s="21"/>
       <c r="V10" s="21"/>
       <c r="W10" s="21"/>
       <c r="X10" s="21"/>
-      <c r="Y10" s="125" t="s">
+      <c r="Y10" s="84" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z10" s="57"/>
+      <c r="AA10" s="57"/>
+      <c r="AB10" s="57"/>
+      <c r="AC10" s="58"/>
+      <c r="AD10" s="78">
+        <v>5</v>
+      </c>
+      <c r="AE10" s="57"/>
+      <c r="AF10" s="57"/>
+      <c r="AG10" s="58"/>
+      <c r="AH10" s="21"/>
+      <c r="AI10" s="21"/>
+      <c r="AJ10" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="Z10" s="61"/>
-      <c r="AA10" s="61"/>
-      <c r="AB10" s="61"/>
-      <c r="AC10" s="62"/>
-      <c r="AD10" s="119">
-        <v>5</v>
-      </c>
-      <c r="AE10" s="61"/>
-      <c r="AF10" s="61"/>
-      <c r="AG10" s="62"/>
-      <c r="AH10" s="21"/>
-      <c r="AI10" s="21"/>
-      <c r="AJ10" s="119" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK10" s="61"/>
-      <c r="AL10" s="61"/>
-      <c r="AM10" s="61"/>
-      <c r="AN10" s="61"/>
-      <c r="AO10" s="117"/>
+      <c r="AK10" s="57"/>
+      <c r="AL10" s="57"/>
+      <c r="AM10" s="57"/>
+      <c r="AN10" s="57"/>
+      <c r="AO10" s="79"/>
       <c r="AP10" s="9"/>
       <c r="AQ10" s="1"/>
       <c r="AR10" s="1"/>
@@ -2362,7 +2365,7 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -2371,11 +2374,11 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="128">
+      <c r="L11" s="71">
         <v>23233</v>
       </c>
-      <c r="M11" s="61"/>
-      <c r="N11" s="62"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="58"/>
       <c r="O11" s="16"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="20">
@@ -2383,22 +2386,22 @@
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
-      <c r="Y11" s="126">
+      <c r="Y11" s="85">
         <v>23060</v>
       </c>
-      <c r="Z11" s="61"/>
-      <c r="AA11" s="61"/>
-      <c r="AB11" s="61"/>
-      <c r="AC11" s="62"/>
-      <c r="AD11" s="120" t="s">
-        <v>28</v>
+      <c r="Z11" s="57"/>
+      <c r="AA11" s="57"/>
+      <c r="AB11" s="57"/>
+      <c r="AC11" s="58"/>
+      <c r="AD11" s="72" t="s">
+        <v>27</v>
       </c>
       <c r="AE11" s="73"/>
       <c r="AF11" s="73"/>
@@ -2410,7 +2413,7 @@
       <c r="AL11" s="73"/>
       <c r="AM11" s="73"/>
       <c r="AN11" s="73"/>
-      <c r="AO11" s="79"/>
+      <c r="AO11" s="74"/>
       <c r="AP11" s="9"/>
       <c r="AQ11" s="1"/>
       <c r="AR11" s="1"/>
@@ -2439,14 +2442,14 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="122"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="62"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="58"/>
       <c r="K12" s="1"/>
       <c r="L12" s="22">
         <v>5</v>
@@ -2460,40 +2463,40 @@
       </c>
       <c r="R12" s="1"/>
       <c r="S12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
-      <c r="Y12" s="126" t="s">
-        <v>31</v>
+      <c r="Y12" s="85" t="s">
+        <v>30</v>
       </c>
-      <c r="Z12" s="61"/>
-      <c r="AA12" s="61"/>
-      <c r="AB12" s="62"/>
+      <c r="Z12" s="57"/>
+      <c r="AA12" s="57"/>
+      <c r="AB12" s="58"/>
       <c r="AC12" s="24"/>
-      <c r="AD12" s="82"/>
-      <c r="AE12" s="83"/>
-      <c r="AF12" s="83"/>
-      <c r="AG12" s="83"/>
-      <c r="AH12" s="83"/>
-      <c r="AI12" s="83"/>
-      <c r="AJ12" s="83"/>
-      <c r="AK12" s="83"/>
-      <c r="AL12" s="83"/>
-      <c r="AM12" s="83"/>
-      <c r="AN12" s="83"/>
-      <c r="AO12" s="85"/>
+      <c r="AD12" s="75"/>
+      <c r="AE12" s="76"/>
+      <c r="AF12" s="76"/>
+      <c r="AG12" s="76"/>
+      <c r="AH12" s="76"/>
+      <c r="AI12" s="76"/>
+      <c r="AJ12" s="76"/>
+      <c r="AK12" s="76"/>
+      <c r="AL12" s="76"/>
+      <c r="AM12" s="76"/>
+      <c r="AN12" s="76"/>
+      <c r="AO12" s="77"/>
       <c r="AP12" s="9"/>
       <c r="AQ12" s="1"/>
-      <c r="AR12" s="63"/>
-      <c r="AS12" s="61"/>
-      <c r="AT12" s="61"/>
-      <c r="AU12" s="61"/>
-      <c r="AV12" s="61"/>
-      <c r="AW12" s="62"/>
+      <c r="AR12" s="80"/>
+      <c r="AS12" s="57"/>
+      <c r="AT12" s="57"/>
+      <c r="AU12" s="57"/>
+      <c r="AV12" s="57"/>
+      <c r="AW12" s="58"/>
       <c r="AX12" s="1"/>
       <c r="AY12" s="1"/>
       <c r="AZ12" s="1"/>
@@ -2514,49 +2517,49 @@
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="129">
+      <c r="H13" s="59">
         <v>45807</v>
       </c>
-      <c r="I13" s="114"/>
-      <c r="J13" s="115"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="61"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
-      <c r="M13" s="130">
+      <c r="M13" s="62">
         <v>9</v>
       </c>
-      <c r="N13" s="114"/>
-      <c r="O13" s="115"/>
+      <c r="N13" s="60"/>
+      <c r="O13" s="61"/>
       <c r="P13" s="13"/>
       <c r="Q13" s="25">
         <v>2.6</v>
       </c>
       <c r="R13" s="13"/>
       <c r="S13" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="T13" s="13"/>
       <c r="U13" s="13"/>
       <c r="V13" s="13"/>
       <c r="W13" s="13"/>
       <c r="X13" s="13"/>
-      <c r="Y13" s="127" t="s">
-        <v>35</v>
+      <c r="Y13" s="68" t="s">
+        <v>34</v>
       </c>
-      <c r="Z13" s="111"/>
-      <c r="AA13" s="111"/>
-      <c r="AB13" s="111"/>
-      <c r="AC13" s="111"/>
-      <c r="AD13" s="111"/>
-      <c r="AE13" s="111"/>
-      <c r="AF13" s="111"/>
-      <c r="AG13" s="111"/>
+      <c r="Z13" s="69"/>
+      <c r="AA13" s="69"/>
+      <c r="AB13" s="69"/>
+      <c r="AC13" s="69"/>
+      <c r="AD13" s="69"/>
+      <c r="AE13" s="69"/>
+      <c r="AF13" s="69"/>
+      <c r="AG13" s="69"/>
       <c r="AH13" s="13"/>
       <c r="AI13" s="13"/>
       <c r="AJ13" s="13"/>
@@ -2656,7 +2659,7 @@
       </c>
       <c r="C15" s="29"/>
       <c r="D15" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" s="29"/>
       <c r="F15" s="29"/>
@@ -2666,16 +2669,16 @@
       <c r="J15" s="29"/>
       <c r="K15" s="29"/>
       <c r="L15" s="29"/>
-      <c r="M15" s="131"/>
-      <c r="N15" s="106"/>
-      <c r="O15" s="57"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="64"/>
+      <c r="O15" s="65"/>
       <c r="P15" s="29"/>
       <c r="Q15" s="31">
         <v>3</v>
       </c>
       <c r="R15" s="29"/>
       <c r="S15" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T15" s="29"/>
       <c r="U15" s="29"/>
@@ -2690,14 +2693,14 @@
       <c r="AD15" s="29"/>
       <c r="AE15" s="29"/>
       <c r="AF15" s="29"/>
-      <c r="AG15" s="56"/>
-      <c r="AH15" s="57"/>
-      <c r="AI15" s="56"/>
-      <c r="AJ15" s="57"/>
-      <c r="AK15" s="56"/>
-      <c r="AL15" s="57"/>
-      <c r="AM15" s="56"/>
-      <c r="AN15" s="57"/>
+      <c r="AG15" s="70"/>
+      <c r="AH15" s="65"/>
+      <c r="AI15" s="70"/>
+      <c r="AJ15" s="65"/>
+      <c r="AK15" s="70"/>
+      <c r="AL15" s="65"/>
+      <c r="AM15" s="70"/>
+      <c r="AN15" s="65"/>
       <c r="AO15" s="32"/>
       <c r="AP15" s="9"/>
       <c r="AQ15" s="1"/>
@@ -2727,54 +2730,54 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="86" t="s">
-        <v>39</v>
+      <c r="H16" s="67" t="s">
+        <v>38</v>
       </c>
-      <c r="I16" s="61"/>
-      <c r="J16" s="61"/>
-      <c r="K16" s="61"/>
-      <c r="L16" s="62"/>
-      <c r="M16" s="87"/>
-      <c r="N16" s="61"/>
-      <c r="O16" s="62"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="57"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="66"/>
+      <c r="N16" s="57"/>
+      <c r="O16" s="58"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="20">
         <v>3.1</v>
       </c>
       <c r="R16" s="1"/>
-      <c r="S16" s="58" t="s">
+      <c r="S16" s="132" t="s">
+        <v>39</v>
+      </c>
+      <c r="T16" s="133"/>
+      <c r="U16" s="133"/>
+      <c r="V16" s="133"/>
+      <c r="W16" s="133"/>
+      <c r="X16" s="133"/>
+      <c r="Y16" s="133"/>
+      <c r="Z16" s="133"/>
+      <c r="AA16" s="133"/>
+      <c r="AB16" s="133"/>
+      <c r="AC16" s="33"/>
+      <c r="AD16" s="33"/>
+      <c r="AE16" s="134" t="s">
         <v>40</v>
       </c>
-      <c r="T16" s="59"/>
-      <c r="U16" s="59"/>
-      <c r="V16" s="59"/>
-      <c r="W16" s="59"/>
-      <c r="X16" s="59"/>
-      <c r="Y16" s="59"/>
-      <c r="Z16" s="59"/>
-      <c r="AA16" s="59"/>
-      <c r="AB16" s="59"/>
-      <c r="AC16" s="33"/>
-      <c r="AD16" s="33"/>
-      <c r="AE16" s="60" t="s">
+      <c r="AF16" s="57"/>
+      <c r="AG16" s="57"/>
+      <c r="AH16" s="58"/>
+      <c r="AI16" s="34"/>
+      <c r="AJ16" s="34"/>
+      <c r="AK16" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="AF16" s="61"/>
-      <c r="AG16" s="61"/>
-      <c r="AH16" s="62"/>
-      <c r="AI16" s="34"/>
-      <c r="AJ16" s="34"/>
-      <c r="AK16" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL16" s="61"/>
-      <c r="AM16" s="61"/>
-      <c r="AN16" s="62"/>
+      <c r="AL16" s="57"/>
+      <c r="AM16" s="57"/>
+      <c r="AN16" s="58"/>
       <c r="AO16" s="35"/>
       <c r="AP16" s="9"/>
       <c r="AQ16" s="1"/>
@@ -2804,54 +2807,54 @@
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="63">
+      <c r="H17" s="80">
         <v>1751</v>
       </c>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="62"/>
-      <c r="M17" s="87"/>
-      <c r="N17" s="61"/>
-      <c r="O17" s="62"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="57"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="66"/>
+      <c r="N17" s="57"/>
+      <c r="O17" s="58"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="20">
         <v>3.2</v>
       </c>
       <c r="R17" s="1"/>
-      <c r="S17" s="64" t="s">
-        <v>44</v>
+      <c r="S17" s="125" t="s">
+        <v>43</v>
       </c>
-      <c r="T17" s="61"/>
-      <c r="U17" s="61"/>
-      <c r="V17" s="61"/>
-      <c r="W17" s="61"/>
-      <c r="X17" s="61"/>
-      <c r="Y17" s="61"/>
-      <c r="Z17" s="61"/>
-      <c r="AA17" s="61"/>
-      <c r="AB17" s="61"/>
-      <c r="AC17" s="62"/>
+      <c r="T17" s="57"/>
+      <c r="U17" s="57"/>
+      <c r="V17" s="57"/>
+      <c r="W17" s="57"/>
+      <c r="X17" s="57"/>
+      <c r="Y17" s="57"/>
+      <c r="Z17" s="57"/>
+      <c r="AA17" s="57"/>
+      <c r="AB17" s="57"/>
+      <c r="AC17" s="58"/>
       <c r="AD17" s="33"/>
-      <c r="AE17" s="60" t="s">
+      <c r="AE17" s="134" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF17" s="57"/>
+      <c r="AG17" s="57"/>
+      <c r="AH17" s="58"/>
+      <c r="AI17" s="33"/>
+      <c r="AJ17" s="33"/>
+      <c r="AK17" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="AF17" s="61"/>
-      <c r="AG17" s="61"/>
-      <c r="AH17" s="62"/>
-      <c r="AI17" s="33"/>
-      <c r="AJ17" s="33"/>
-      <c r="AK17" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL17" s="61"/>
-      <c r="AM17" s="61"/>
-      <c r="AN17" s="62"/>
+      <c r="AL17" s="57"/>
+      <c r="AM17" s="57"/>
+      <c r="AN17" s="58"/>
       <c r="AO17" s="35"/>
       <c r="AP17" s="9"/>
       <c r="AQ17" s="1"/>
@@ -2881,54 +2884,54 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="109" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="88" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
-      <c r="H18" s="61"/>
-      <c r="I18" s="61"/>
-      <c r="J18" s="61"/>
-      <c r="K18" s="61"/>
-      <c r="L18" s="61"/>
-      <c r="M18" s="61"/>
-      <c r="N18" s="61"/>
-      <c r="O18" s="61"/>
-      <c r="P18" s="62"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="57"/>
+      <c r="O18" s="57"/>
+      <c r="P18" s="58"/>
       <c r="Q18" s="20">
         <v>3.3</v>
       </c>
       <c r="R18" s="1"/>
-      <c r="S18" s="64" t="s">
+      <c r="S18" s="125" t="s">
+        <v>46</v>
+      </c>
+      <c r="T18" s="57"/>
+      <c r="U18" s="57"/>
+      <c r="V18" s="57"/>
+      <c r="W18" s="57"/>
+      <c r="X18" s="57"/>
+      <c r="Y18" s="57"/>
+      <c r="Z18" s="57"/>
+      <c r="AA18" s="57"/>
+      <c r="AB18" s="57"/>
+      <c r="AC18" s="58"/>
+      <c r="AD18" s="33"/>
+      <c r="AE18" s="129" t="s">
         <v>47</v>
       </c>
-      <c r="T18" s="61"/>
-      <c r="U18" s="61"/>
-      <c r="V18" s="61"/>
-      <c r="W18" s="61"/>
-      <c r="X18" s="61"/>
-      <c r="Y18" s="61"/>
-      <c r="Z18" s="61"/>
-      <c r="AA18" s="61"/>
-      <c r="AB18" s="61"/>
-      <c r="AC18" s="62"/>
-      <c r="AD18" s="33"/>
-      <c r="AE18" s="65" t="s">
+      <c r="AF18" s="57"/>
+      <c r="AG18" s="57"/>
+      <c r="AH18" s="58"/>
+      <c r="AI18" s="33"/>
+      <c r="AJ18" s="33"/>
+      <c r="AK18" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="AF18" s="61"/>
-      <c r="AG18" s="61"/>
-      <c r="AH18" s="62"/>
-      <c r="AI18" s="33"/>
-      <c r="AJ18" s="33"/>
-      <c r="AK18" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="AL18" s="61"/>
-      <c r="AM18" s="61"/>
-      <c r="AN18" s="62"/>
+      <c r="AL18" s="57"/>
+      <c r="AM18" s="57"/>
+      <c r="AN18" s="58"/>
       <c r="AO18" s="35"/>
       <c r="AP18" s="9"/>
       <c r="AQ18" s="1"/>
@@ -2958,52 +2961,52 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="63">
+      <c r="H19" s="80">
         <v>238350</v>
       </c>
-      <c r="I19" s="61"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="61"/>
-      <c r="L19" s="62"/>
-      <c r="M19" s="87"/>
-      <c r="N19" s="61"/>
-      <c r="O19" s="62"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="66"/>
+      <c r="N19" s="57"/>
+      <c r="O19" s="58"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="20">
         <v>3.4</v>
       </c>
       <c r="R19" s="1"/>
-      <c r="S19" s="64" t="s">
-        <v>51</v>
+      <c r="S19" s="125" t="s">
+        <v>50</v>
       </c>
-      <c r="T19" s="61"/>
-      <c r="U19" s="61"/>
-      <c r="V19" s="61"/>
-      <c r="W19" s="61"/>
-      <c r="X19" s="61"/>
-      <c r="Y19" s="61"/>
-      <c r="Z19" s="61"/>
-      <c r="AA19" s="61"/>
-      <c r="AB19" s="61"/>
-      <c r="AC19" s="62"/>
+      <c r="T19" s="57"/>
+      <c r="U19" s="57"/>
+      <c r="V19" s="57"/>
+      <c r="W19" s="57"/>
+      <c r="X19" s="57"/>
+      <c r="Y19" s="57"/>
+      <c r="Z19" s="57"/>
+      <c r="AA19" s="57"/>
+      <c r="AB19" s="57"/>
+      <c r="AC19" s="58"/>
       <c r="AD19" s="33"/>
-      <c r="AE19" s="132">
+      <c r="AE19" s="131">
         <v>25000</v>
       </c>
-      <c r="AF19" s="61"/>
-      <c r="AG19" s="61"/>
-      <c r="AH19" s="62"/>
+      <c r="AF19" s="57"/>
+      <c r="AG19" s="57"/>
+      <c r="AH19" s="58"/>
       <c r="AI19" s="33"/>
       <c r="AJ19" s="33"/>
-      <c r="AK19" s="63"/>
-      <c r="AL19" s="61"/>
-      <c r="AM19" s="61"/>
-      <c r="AN19" s="62"/>
+      <c r="AK19" s="80"/>
+      <c r="AL19" s="57"/>
+      <c r="AM19" s="57"/>
+      <c r="AN19" s="58"/>
       <c r="AO19" s="35"/>
       <c r="AP19" s="9"/>
       <c r="AQ19" s="1"/>
@@ -3033,54 +3036,54 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="109" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="88" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="61"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="61"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="61"/>
-      <c r="L20" s="61"/>
-      <c r="M20" s="61"/>
-      <c r="N20" s="61"/>
-      <c r="O20" s="61"/>
-      <c r="P20" s="62"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="57"/>
+      <c r="K20" s="57"/>
+      <c r="L20" s="57"/>
+      <c r="M20" s="57"/>
+      <c r="N20" s="57"/>
+      <c r="O20" s="57"/>
+      <c r="P20" s="58"/>
       <c r="Q20" s="36">
         <v>3.5</v>
       </c>
       <c r="R20" s="14"/>
-      <c r="S20" s="64" t="s">
-        <v>54</v>
+      <c r="S20" s="125" t="s">
+        <v>53</v>
       </c>
-      <c r="T20" s="61"/>
-      <c r="U20" s="61"/>
-      <c r="V20" s="61"/>
-      <c r="W20" s="61"/>
-      <c r="X20" s="61"/>
-      <c r="Y20" s="61"/>
-      <c r="Z20" s="61"/>
-      <c r="AA20" s="61"/>
-      <c r="AB20" s="61"/>
-      <c r="AC20" s="62"/>
+      <c r="T20" s="57"/>
+      <c r="U20" s="57"/>
+      <c r="V20" s="57"/>
+      <c r="W20" s="57"/>
+      <c r="X20" s="57"/>
+      <c r="Y20" s="57"/>
+      <c r="Z20" s="57"/>
+      <c r="AA20" s="57"/>
+      <c r="AB20" s="57"/>
+      <c r="AC20" s="58"/>
       <c r="AD20" s="33"/>
-      <c r="AE20" s="65" t="s">
+      <c r="AE20" s="129" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF20" s="57"/>
+      <c r="AG20" s="57"/>
+      <c r="AH20" s="58"/>
+      <c r="AI20" s="33"/>
+      <c r="AJ20" s="33"/>
+      <c r="AK20" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="AF20" s="61"/>
-      <c r="AG20" s="61"/>
-      <c r="AH20" s="62"/>
-      <c r="AI20" s="33"/>
-      <c r="AJ20" s="33"/>
-      <c r="AK20" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL20" s="61"/>
-      <c r="AM20" s="61"/>
-      <c r="AN20" s="62"/>
+      <c r="AL20" s="57"/>
+      <c r="AM20" s="57"/>
+      <c r="AN20" s="58"/>
       <c r="AO20" s="35"/>
       <c r="AP20" s="9"/>
       <c r="AQ20" s="1"/>
@@ -3110,50 +3113,50 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E21" s="37"/>
       <c r="F21" s="37"/>
       <c r="G21" s="37"/>
-      <c r="H21" s="133">
+      <c r="H21" s="112">
         <v>45839</v>
       </c>
-      <c r="I21" s="61"/>
-      <c r="J21" s="62"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="58"/>
       <c r="K21" s="37"/>
       <c r="L21" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
-      <c r="M21" s="100">
+      <c r="M21" s="108">
         <v>41</v>
       </c>
-      <c r="N21" s="61"/>
-      <c r="O21" s="62"/>
+      <c r="N21" s="57"/>
+      <c r="O21" s="58"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="20"/>
       <c r="R21" s="1"/>
-      <c r="S21" s="134" t="s">
-        <v>57</v>
+      <c r="S21" s="130" t="s">
+        <v>56</v>
       </c>
-      <c r="T21" s="61"/>
-      <c r="U21" s="61"/>
-      <c r="V21" s="61"/>
-      <c r="W21" s="61"/>
-      <c r="X21" s="61"/>
-      <c r="Y21" s="61"/>
-      <c r="Z21" s="61"/>
-      <c r="AA21" s="61"/>
-      <c r="AB21" s="61"/>
-      <c r="AC21" s="61"/>
-      <c r="AD21" s="61"/>
-      <c r="AE21" s="61"/>
-      <c r="AF21" s="61"/>
-      <c r="AG21" s="61"/>
-      <c r="AH21" s="61"/>
-      <c r="AI21" s="61"/>
-      <c r="AJ21" s="61"/>
-      <c r="AK21" s="61"/>
-      <c r="AL21" s="62"/>
+      <c r="T21" s="57"/>
+      <c r="U21" s="57"/>
+      <c r="V21" s="57"/>
+      <c r="W21" s="57"/>
+      <c r="X21" s="57"/>
+      <c r="Y21" s="57"/>
+      <c r="Z21" s="57"/>
+      <c r="AA21" s="57"/>
+      <c r="AB21" s="57"/>
+      <c r="AC21" s="57"/>
+      <c r="AD21" s="57"/>
+      <c r="AE21" s="57"/>
+      <c r="AF21" s="57"/>
+      <c r="AG21" s="57"/>
+      <c r="AH21" s="57"/>
+      <c r="AI21" s="57"/>
+      <c r="AJ21" s="57"/>
+      <c r="AK21" s="57"/>
+      <c r="AL21" s="58"/>
       <c r="AM21" s="1"/>
       <c r="AN21" s="1"/>
       <c r="AO21" s="27"/>
@@ -3185,56 +3188,56 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="97">
+      <c r="H22" s="105">
         <v>200000</v>
       </c>
-      <c r="I22" s="61"/>
-      <c r="J22" s="62"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="58"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
-      <c r="M22" s="98">
+      <c r="M22" s="106">
         <v>50</v>
       </c>
-      <c r="N22" s="61"/>
-      <c r="O22" s="62"/>
+      <c r="N22" s="57"/>
+      <c r="O22" s="58"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="36">
         <v>3.6</v>
       </c>
       <c r="R22" s="1"/>
-      <c r="S22" s="67" t="s">
-        <v>60</v>
+      <c r="S22" s="126" t="s">
+        <v>59</v>
       </c>
-      <c r="T22" s="61"/>
-      <c r="U22" s="61"/>
-      <c r="V22" s="61"/>
-      <c r="W22" s="61"/>
-      <c r="X22" s="61"/>
-      <c r="Y22" s="61"/>
-      <c r="Z22" s="61"/>
-      <c r="AA22" s="61"/>
-      <c r="AB22" s="61"/>
-      <c r="AC22" s="61"/>
-      <c r="AD22" s="61"/>
-      <c r="AE22" s="61"/>
-      <c r="AF22" s="61"/>
-      <c r="AG22" s="61"/>
-      <c r="AH22" s="62"/>
+      <c r="T22" s="57"/>
+      <c r="U22" s="57"/>
+      <c r="V22" s="57"/>
+      <c r="W22" s="57"/>
+      <c r="X22" s="57"/>
+      <c r="Y22" s="57"/>
+      <c r="Z22" s="57"/>
+      <c r="AA22" s="57"/>
+      <c r="AB22" s="57"/>
+      <c r="AC22" s="57"/>
+      <c r="AD22" s="57"/>
+      <c r="AE22" s="57"/>
+      <c r="AF22" s="57"/>
+      <c r="AG22" s="57"/>
+      <c r="AH22" s="58"/>
       <c r="AI22" s="39"/>
       <c r="AJ22" s="39"/>
-      <c r="AK22" s="63">
+      <c r="AK22" s="80">
         <v>5</v>
       </c>
-      <c r="AL22" s="61"/>
-      <c r="AM22" s="61"/>
-      <c r="AN22" s="62"/>
+      <c r="AL22" s="57"/>
+      <c r="AM22" s="57"/>
+      <c r="AN22" s="58"/>
       <c r="AO22" s="40"/>
       <c r="AP22" s="9"/>
       <c r="AQ22" s="1"/>
@@ -3264,56 +3267,56 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="99">
+      <c r="H23" s="107">
         <v>5000000</v>
       </c>
-      <c r="I23" s="61"/>
-      <c r="J23" s="62"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="58"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
-      <c r="M23" s="98">
+      <c r="M23" s="106">
         <v>60</v>
       </c>
-      <c r="N23" s="61"/>
-      <c r="O23" s="62"/>
+      <c r="N23" s="57"/>
+      <c r="O23" s="58"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="36">
         <v>3.7</v>
       </c>
       <c r="R23" s="1"/>
-      <c r="S23" s="68" t="s">
-        <v>63</v>
+      <c r="S23" s="127" t="s">
+        <v>62</v>
       </c>
-      <c r="T23" s="61"/>
-      <c r="U23" s="61"/>
-      <c r="V23" s="61"/>
-      <c r="W23" s="61"/>
-      <c r="X23" s="61"/>
-      <c r="Y23" s="61"/>
-      <c r="Z23" s="61"/>
-      <c r="AA23" s="61"/>
-      <c r="AB23" s="61"/>
-      <c r="AC23" s="61"/>
-      <c r="AD23" s="61"/>
-      <c r="AE23" s="61"/>
-      <c r="AF23" s="61"/>
-      <c r="AG23" s="61"/>
-      <c r="AH23" s="62"/>
+      <c r="T23" s="57"/>
+      <c r="U23" s="57"/>
+      <c r="V23" s="57"/>
+      <c r="W23" s="57"/>
+      <c r="X23" s="57"/>
+      <c r="Y23" s="57"/>
+      <c r="Z23" s="57"/>
+      <c r="AA23" s="57"/>
+      <c r="AB23" s="57"/>
+      <c r="AC23" s="57"/>
+      <c r="AD23" s="57"/>
+      <c r="AE23" s="57"/>
+      <c r="AF23" s="57"/>
+      <c r="AG23" s="57"/>
+      <c r="AH23" s="58"/>
       <c r="AI23" s="1"/>
       <c r="AJ23" s="1"/>
-      <c r="AK23" s="69">
+      <c r="AK23" s="128">
         <v>14500</v>
       </c>
-      <c r="AL23" s="61"/>
-      <c r="AM23" s="61"/>
-      <c r="AN23" s="62"/>
+      <c r="AL23" s="57"/>
+      <c r="AM23" s="57"/>
+      <c r="AN23" s="58"/>
       <c r="AO23" s="27"/>
       <c r="AP23" s="9"/>
       <c r="AQ23" s="1"/>
@@ -3343,54 +3346,54 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="99">
+      <c r="H24" s="107">
         <v>10000000</v>
       </c>
-      <c r="I24" s="61"/>
-      <c r="J24" s="62"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="58"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
-      <c r="M24" s="100"/>
-      <c r="N24" s="61"/>
-      <c r="O24" s="62"/>
+      <c r="M24" s="108"/>
+      <c r="N24" s="57"/>
+      <c r="O24" s="58"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="36">
         <v>3.8</v>
       </c>
       <c r="R24" s="1"/>
-      <c r="S24" s="68" t="s">
-        <v>66</v>
+      <c r="S24" s="127" t="s">
+        <v>65</v>
       </c>
-      <c r="T24" s="61"/>
-      <c r="U24" s="61"/>
-      <c r="V24" s="61"/>
-      <c r="W24" s="61"/>
-      <c r="X24" s="61"/>
-      <c r="Y24" s="61"/>
-      <c r="Z24" s="61"/>
-      <c r="AA24" s="61"/>
-      <c r="AB24" s="61"/>
-      <c r="AC24" s="61"/>
-      <c r="AD24" s="61"/>
-      <c r="AE24" s="61"/>
-      <c r="AF24" s="61"/>
-      <c r="AG24" s="61"/>
-      <c r="AH24" s="62"/>
+      <c r="T24" s="57"/>
+      <c r="U24" s="57"/>
+      <c r="V24" s="57"/>
+      <c r="W24" s="57"/>
+      <c r="X24" s="57"/>
+      <c r="Y24" s="57"/>
+      <c r="Z24" s="57"/>
+      <c r="AA24" s="57"/>
+      <c r="AB24" s="57"/>
+      <c r="AC24" s="57"/>
+      <c r="AD24" s="57"/>
+      <c r="AE24" s="57"/>
+      <c r="AF24" s="57"/>
+      <c r="AG24" s="57"/>
+      <c r="AH24" s="58"/>
       <c r="AI24" s="1"/>
       <c r="AJ24" s="1"/>
-      <c r="AK24" s="66">
+      <c r="AK24" s="124">
         <v>0.79</v>
       </c>
-      <c r="AL24" s="61"/>
-      <c r="AM24" s="61"/>
-      <c r="AN24" s="62"/>
+      <c r="AL24" s="57"/>
+      <c r="AM24" s="57"/>
+      <c r="AN24" s="58"/>
       <c r="AO24" s="27"/>
       <c r="AP24" s="9"/>
       <c r="AQ24" s="1"/>
@@ -3426,40 +3429,40 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="43"/>
-      <c r="M25" s="63"/>
-      <c r="N25" s="61"/>
-      <c r="O25" s="62"/>
+      <c r="M25" s="80"/>
+      <c r="N25" s="57"/>
+      <c r="O25" s="58"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="36">
         <v>3.9</v>
       </c>
       <c r="R25" s="1"/>
-      <c r="S25" s="68" t="s">
-        <v>67</v>
+      <c r="S25" s="127" t="s">
+        <v>66</v>
       </c>
-      <c r="T25" s="61"/>
-      <c r="U25" s="61"/>
-      <c r="V25" s="61"/>
-      <c r="W25" s="61"/>
-      <c r="X25" s="61"/>
-      <c r="Y25" s="61"/>
-      <c r="Z25" s="61"/>
-      <c r="AA25" s="61"/>
-      <c r="AB25" s="61"/>
-      <c r="AC25" s="61"/>
-      <c r="AD25" s="61"/>
-      <c r="AE25" s="61"/>
-      <c r="AF25" s="61"/>
-      <c r="AG25" s="61"/>
-      <c r="AH25" s="62"/>
+      <c r="T25" s="57"/>
+      <c r="U25" s="57"/>
+      <c r="V25" s="57"/>
+      <c r="W25" s="57"/>
+      <c r="X25" s="57"/>
+      <c r="Y25" s="57"/>
+      <c r="Z25" s="57"/>
+      <c r="AA25" s="57"/>
+      <c r="AB25" s="57"/>
+      <c r="AC25" s="57"/>
+      <c r="AD25" s="57"/>
+      <c r="AE25" s="57"/>
+      <c r="AF25" s="57"/>
+      <c r="AG25" s="57"/>
+      <c r="AH25" s="58"/>
       <c r="AI25" s="1"/>
       <c r="AJ25" s="1"/>
-      <c r="AK25" s="63">
+      <c r="AK25" s="80">
         <v>29</v>
       </c>
-      <c r="AL25" s="61"/>
-      <c r="AM25" s="61"/>
-      <c r="AN25" s="62"/>
+      <c r="AL25" s="57"/>
+      <c r="AM25" s="57"/>
+      <c r="AN25" s="58"/>
       <c r="AO25" s="27"/>
       <c r="AP25" s="9"/>
       <c r="AQ25" s="1"/>
@@ -3489,7 +3492,7 @@
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
@@ -3508,7 +3511,7 @@
       </c>
       <c r="R26" s="18"/>
       <c r="S26" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T26" s="18"/>
       <c r="U26" s="18"/>
@@ -3560,7 +3563,7 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -3570,52 +3573,52 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
-      <c r="M27" s="89" t="s">
-        <v>48</v>
+      <c r="M27" s="110" t="s">
+        <v>47</v>
       </c>
-      <c r="N27" s="90"/>
-      <c r="O27" s="91"/>
+      <c r="N27" s="100"/>
+      <c r="O27" s="101"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="20">
         <v>6.1</v>
       </c>
       <c r="R27" s="1"/>
-      <c r="S27" s="81" t="s">
+      <c r="S27" s="122" t="s">
+        <v>70</v>
+      </c>
+      <c r="T27" s="57"/>
+      <c r="U27" s="57"/>
+      <c r="V27" s="57"/>
+      <c r="W27" s="57"/>
+      <c r="X27" s="57"/>
+      <c r="Y27" s="58"/>
+      <c r="Z27" s="113">
+        <v>78</v>
+      </c>
+      <c r="AA27" s="57"/>
+      <c r="AB27" s="58"/>
+      <c r="AC27" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="T27" s="61"/>
-      <c r="U27" s="61"/>
-      <c r="V27" s="61"/>
-      <c r="W27" s="61"/>
-      <c r="X27" s="61"/>
-      <c r="Y27" s="62"/>
-      <c r="Z27" s="70">
-        <v>78</v>
+      <c r="AD27" s="46" t="s">
+        <v>71</v>
       </c>
-      <c r="AA27" s="61"/>
-      <c r="AB27" s="62"/>
-      <c r="AC27" s="46" t="s">
+      <c r="AE27" s="122" t="s">
         <v>72</v>
       </c>
-      <c r="AD27" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE27" s="81" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF27" s="61"/>
-      <c r="AG27" s="61"/>
-      <c r="AH27" s="61"/>
-      <c r="AI27" s="61"/>
-      <c r="AJ27" s="61"/>
-      <c r="AK27" s="62"/>
-      <c r="AL27" s="70">
+      <c r="AF27" s="57"/>
+      <c r="AG27" s="57"/>
+      <c r="AH27" s="57"/>
+      <c r="AI27" s="57"/>
+      <c r="AJ27" s="57"/>
+      <c r="AK27" s="58"/>
+      <c r="AL27" s="113">
         <v>89</v>
       </c>
-      <c r="AM27" s="61"/>
-      <c r="AN27" s="62"/>
+      <c r="AM27" s="57"/>
+      <c r="AN27" s="58"/>
       <c r="AO27" s="47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AP27" s="9"/>
       <c r="AQ27" s="1"/>
@@ -3645,7 +3648,7 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -3655,18 +3658,18 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
-      <c r="M28" s="89" t="s">
-        <v>48</v>
+      <c r="M28" s="110" t="s">
+        <v>47</v>
       </c>
-      <c r="N28" s="90"/>
-      <c r="O28" s="91"/>
+      <c r="N28" s="100"/>
+      <c r="O28" s="101"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="20">
         <v>6.2</v>
       </c>
       <c r="R28" s="1"/>
-      <c r="S28" s="78" t="s">
-        <v>75</v>
+      <c r="S28" s="120" t="s">
+        <v>74</v>
       </c>
       <c r="T28" s="73"/>
       <c r="U28" s="73"/>
@@ -3677,12 +3680,12 @@
       <c r="Z28" s="73"/>
       <c r="AA28" s="73"/>
       <c r="AB28" s="73"/>
-      <c r="AC28" s="74"/>
+      <c r="AC28" s="116"/>
       <c r="AD28" s="46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
-      <c r="AE28" s="78" t="s">
-        <v>76</v>
+      <c r="AE28" s="120" t="s">
+        <v>75</v>
       </c>
       <c r="AF28" s="73"/>
       <c r="AG28" s="73"/>
@@ -3693,7 +3696,7 @@
       <c r="AL28" s="73"/>
       <c r="AM28" s="73"/>
       <c r="AN28" s="73"/>
-      <c r="AO28" s="79"/>
+      <c r="AO28" s="74"/>
       <c r="AP28" s="9"/>
       <c r="AQ28" s="1"/>
       <c r="AR28" s="1"/>
@@ -3722,7 +3725,7 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -3731,40 +3734,40 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
-      <c r="L29" s="63"/>
-      <c r="M29" s="61"/>
-      <c r="N29" s="61"/>
-      <c r="O29" s="62"/>
+      <c r="L29" s="80"/>
+      <c r="M29" s="57"/>
+      <c r="N29" s="57"/>
+      <c r="O29" s="58"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="20">
         <v>6.3</v>
       </c>
       <c r="R29" s="1"/>
-      <c r="S29" s="82"/>
-      <c r="T29" s="83"/>
-      <c r="U29" s="83"/>
-      <c r="V29" s="83"/>
-      <c r="W29" s="83"/>
-      <c r="X29" s="83"/>
-      <c r="Y29" s="83"/>
-      <c r="Z29" s="83"/>
-      <c r="AA29" s="83"/>
-      <c r="AB29" s="83"/>
-      <c r="AC29" s="84"/>
+      <c r="S29" s="75"/>
+      <c r="T29" s="76"/>
+      <c r="U29" s="76"/>
+      <c r="V29" s="76"/>
+      <c r="W29" s="76"/>
+      <c r="X29" s="76"/>
+      <c r="Y29" s="76"/>
+      <c r="Z29" s="76"/>
+      <c r="AA29" s="76"/>
+      <c r="AB29" s="76"/>
+      <c r="AC29" s="123"/>
       <c r="AD29" s="46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
-      <c r="AE29" s="82"/>
-      <c r="AF29" s="83"/>
-      <c r="AG29" s="83"/>
-      <c r="AH29" s="83"/>
-      <c r="AI29" s="83"/>
-      <c r="AJ29" s="83"/>
-      <c r="AK29" s="83"/>
-      <c r="AL29" s="83"/>
-      <c r="AM29" s="83"/>
-      <c r="AN29" s="83"/>
-      <c r="AO29" s="85"/>
+      <c r="AE29" s="75"/>
+      <c r="AF29" s="76"/>
+      <c r="AG29" s="76"/>
+      <c r="AH29" s="76"/>
+      <c r="AI29" s="76"/>
+      <c r="AJ29" s="76"/>
+      <c r="AK29" s="76"/>
+      <c r="AL29" s="76"/>
+      <c r="AM29" s="76"/>
+      <c r="AN29" s="76"/>
+      <c r="AO29" s="77"/>
       <c r="AP29" s="9"/>
       <c r="AQ29" s="1"/>
       <c r="AR29" s="1"/>
@@ -3793,7 +3796,7 @@
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -3801,53 +3804,53 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
-      <c r="L30" s="92">
+      <c r="L30" s="111">
         <v>70000</v>
       </c>
-      <c r="M30" s="90"/>
-      <c r="N30" s="90"/>
-      <c r="O30" s="91"/>
+      <c r="M30" s="100"/>
+      <c r="N30" s="100"/>
+      <c r="O30" s="101"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="20">
         <v>6.4</v>
       </c>
       <c r="R30" s="1"/>
-      <c r="S30" s="81" t="s">
+      <c r="S30" s="122" t="s">
+        <v>78</v>
+      </c>
+      <c r="T30" s="57"/>
+      <c r="U30" s="57"/>
+      <c r="V30" s="57"/>
+      <c r="W30" s="57"/>
+      <c r="X30" s="57"/>
+      <c r="Y30" s="58"/>
+      <c r="Z30" s="113">
+        <v>74</v>
+      </c>
+      <c r="AA30" s="57"/>
+      <c r="AB30" s="58"/>
+      <c r="AC30" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD30" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE30" s="114" t="s">
         <v>79</v>
       </c>
-      <c r="T30" s="61"/>
-      <c r="U30" s="61"/>
-      <c r="V30" s="61"/>
-      <c r="W30" s="61"/>
-      <c r="X30" s="61"/>
-      <c r="Y30" s="62"/>
-      <c r="Z30" s="70">
-        <v>74</v>
-      </c>
-      <c r="AA30" s="61"/>
-      <c r="AB30" s="62"/>
-      <c r="AC30" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="AD30" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE30" s="71" t="s">
-        <v>80</v>
-      </c>
-      <c r="AF30" s="61"/>
-      <c r="AG30" s="61"/>
-      <c r="AH30" s="61"/>
-      <c r="AI30" s="61"/>
-      <c r="AJ30" s="61"/>
-      <c r="AK30" s="62"/>
-      <c r="AL30" s="70">
+      <c r="AF30" s="57"/>
+      <c r="AG30" s="57"/>
+      <c r="AH30" s="57"/>
+      <c r="AI30" s="57"/>
+      <c r="AJ30" s="57"/>
+      <c r="AK30" s="58"/>
+      <c r="AL30" s="113">
         <v>15</v>
       </c>
-      <c r="AM30" s="61"/>
-      <c r="AN30" s="62"/>
+      <c r="AM30" s="57"/>
+      <c r="AN30" s="58"/>
       <c r="AO30" s="47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AP30" s="9"/>
       <c r="AQ30" s="1"/>
@@ -3877,7 +3880,7 @@
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -3885,19 +3888,19 @@
       <c r="I31" s="48"/>
       <c r="J31" s="48"/>
       <c r="K31" s="48"/>
-      <c r="L31" s="93">
+      <c r="L31" s="99">
         <v>85000</v>
       </c>
-      <c r="M31" s="90"/>
-      <c r="N31" s="90"/>
-      <c r="O31" s="91"/>
+      <c r="M31" s="100"/>
+      <c r="N31" s="100"/>
+      <c r="O31" s="101"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="20">
         <v>6.5</v>
       </c>
       <c r="R31" s="1"/>
-      <c r="S31" s="72" t="s">
-        <v>82</v>
+      <c r="S31" s="115" t="s">
+        <v>81</v>
       </c>
       <c r="T31" s="73"/>
       <c r="U31" s="73"/>
@@ -3908,12 +3911,12 @@
       <c r="Z31" s="73"/>
       <c r="AA31" s="73"/>
       <c r="AB31" s="73"/>
-      <c r="AC31" s="74"/>
+      <c r="AC31" s="116"/>
       <c r="AD31" s="46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
-      <c r="AE31" s="78" t="s">
-        <v>83</v>
+      <c r="AE31" s="120" t="s">
+        <v>82</v>
       </c>
       <c r="AF31" s="73"/>
       <c r="AG31" s="73"/>
@@ -3924,7 +3927,7 @@
       <c r="AL31" s="73"/>
       <c r="AM31" s="73"/>
       <c r="AN31" s="73"/>
-      <c r="AO31" s="79"/>
+      <c r="AO31" s="74"/>
       <c r="AP31" s="9"/>
       <c r="AQ31" s="1"/>
       <c r="AR31" s="1"/>
@@ -3953,7 +3956,7 @@
       </c>
       <c r="C32" s="50"/>
       <c r="D32" s="50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E32" s="51"/>
       <c r="F32" s="50"/>
@@ -3962,42 +3965,42 @@
       <c r="I32" s="52"/>
       <c r="J32" s="52"/>
       <c r="K32" s="52"/>
-      <c r="L32" s="94">
+      <c r="L32" s="102">
         <v>3</v>
       </c>
-      <c r="M32" s="95"/>
-      <c r="N32" s="95"/>
-      <c r="O32" s="96"/>
+      <c r="M32" s="103"/>
+      <c r="N32" s="103"/>
+      <c r="O32" s="104"/>
       <c r="P32" s="50"/>
       <c r="Q32" s="53">
         <v>6.6</v>
       </c>
       <c r="R32" s="50"/>
-      <c r="S32" s="75"/>
-      <c r="T32" s="76"/>
-      <c r="U32" s="76"/>
-      <c r="V32" s="76"/>
-      <c r="W32" s="76"/>
-      <c r="X32" s="76"/>
-      <c r="Y32" s="76"/>
-      <c r="Z32" s="76"/>
-      <c r="AA32" s="76"/>
-      <c r="AB32" s="76"/>
-      <c r="AC32" s="77"/>
+      <c r="S32" s="117"/>
+      <c r="T32" s="118"/>
+      <c r="U32" s="118"/>
+      <c r="V32" s="118"/>
+      <c r="W32" s="118"/>
+      <c r="X32" s="118"/>
+      <c r="Y32" s="118"/>
+      <c r="Z32" s="118"/>
+      <c r="AA32" s="118"/>
+      <c r="AB32" s="118"/>
+      <c r="AC32" s="119"/>
       <c r="AD32" s="54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
-      <c r="AE32" s="75"/>
-      <c r="AF32" s="76"/>
-      <c r="AG32" s="76"/>
-      <c r="AH32" s="76"/>
-      <c r="AI32" s="76"/>
-      <c r="AJ32" s="76"/>
-      <c r="AK32" s="76"/>
-      <c r="AL32" s="76"/>
-      <c r="AM32" s="76"/>
-      <c r="AN32" s="76"/>
-      <c r="AO32" s="80"/>
+      <c r="AE32" s="117"/>
+      <c r="AF32" s="118"/>
+      <c r="AG32" s="118"/>
+      <c r="AH32" s="118"/>
+      <c r="AI32" s="118"/>
+      <c r="AJ32" s="118"/>
+      <c r="AK32" s="118"/>
+      <c r="AL32" s="118"/>
+      <c r="AM32" s="118"/>
+      <c r="AN32" s="118"/>
+      <c r="AO32" s="121"/>
       <c r="AP32" s="9"/>
       <c r="AQ32" s="1"/>
       <c r="AR32" s="1"/>
@@ -65004,17 +65007,68 @@
     </row>
   </sheetData>
   <mergeCells count="93">
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="Y13:AG13"/>
-    <mergeCell ref="AG15:AH15"/>
-    <mergeCell ref="AI15:AJ15"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="AD11:AO12"/>
+    <mergeCell ref="S16:AB16"/>
+    <mergeCell ref="AE16:AH16"/>
+    <mergeCell ref="AK16:AN16"/>
+    <mergeCell ref="AE17:AH17"/>
+    <mergeCell ref="AK17:AN17"/>
+    <mergeCell ref="S17:AC17"/>
+    <mergeCell ref="S18:AC18"/>
+    <mergeCell ref="AE18:AH18"/>
+    <mergeCell ref="AK18:AN18"/>
+    <mergeCell ref="S19:AC19"/>
+    <mergeCell ref="AK19:AN19"/>
+    <mergeCell ref="AE19:AH19"/>
+    <mergeCell ref="AK20:AN20"/>
+    <mergeCell ref="AK24:AN24"/>
+    <mergeCell ref="AK25:AN25"/>
+    <mergeCell ref="S20:AC20"/>
+    <mergeCell ref="S22:AH22"/>
+    <mergeCell ref="AK22:AN22"/>
+    <mergeCell ref="S23:AH23"/>
+    <mergeCell ref="AK23:AN23"/>
+    <mergeCell ref="S24:AH24"/>
+    <mergeCell ref="S25:AH25"/>
+    <mergeCell ref="AE20:AH20"/>
+    <mergeCell ref="S21:AL21"/>
+    <mergeCell ref="Z30:AB30"/>
+    <mergeCell ref="AE30:AK30"/>
+    <mergeCell ref="S31:AC32"/>
+    <mergeCell ref="AE31:AO32"/>
+    <mergeCell ref="S27:Y27"/>
+    <mergeCell ref="Z27:AB27"/>
+    <mergeCell ref="AE27:AK27"/>
+    <mergeCell ref="AL27:AN27"/>
+    <mergeCell ref="S28:AC29"/>
+    <mergeCell ref="AE28:AO29"/>
+    <mergeCell ref="S30:Y30"/>
+    <mergeCell ref="AL30:AN30"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="E18:P18"/>
+    <mergeCell ref="H19:L19"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="E20:P20"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="L29:O29"/>
+    <mergeCell ref="L30:O30"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="L31:O31"/>
+    <mergeCell ref="L32:O32"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="Y4:AN4"/>
+    <mergeCell ref="D5:J5"/>
+    <mergeCell ref="K5:AO6"/>
+    <mergeCell ref="H6:J6"/>
     <mergeCell ref="AR12:AW12"/>
     <mergeCell ref="L7:N7"/>
     <mergeCell ref="L8:N8"/>
@@ -65031,72 +65085,21 @@
     <mergeCell ref="AJ7:AO7"/>
     <mergeCell ref="AJ8:AO8"/>
     <mergeCell ref="AJ9:AO9"/>
+    <mergeCell ref="Y13:AG13"/>
+    <mergeCell ref="AG15:AH15"/>
+    <mergeCell ref="AI15:AJ15"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="AD11:AO12"/>
     <mergeCell ref="AJ10:AO10"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="Y4:AN4"/>
-    <mergeCell ref="D5:J5"/>
-    <mergeCell ref="K5:AO6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="L31:O31"/>
-    <mergeCell ref="L32:O32"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="E20:P20"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="M28:O28"/>
-    <mergeCell ref="L29:O29"/>
-    <mergeCell ref="L30:O30"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="H16:L16"/>
-    <mergeCell ref="H17:L17"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="E18:P18"/>
-    <mergeCell ref="H19:L19"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="Z30:AB30"/>
-    <mergeCell ref="AE30:AK30"/>
-    <mergeCell ref="S31:AC32"/>
-    <mergeCell ref="AE31:AO32"/>
-    <mergeCell ref="S27:Y27"/>
-    <mergeCell ref="Z27:AB27"/>
-    <mergeCell ref="AE27:AK27"/>
-    <mergeCell ref="AL27:AN27"/>
-    <mergeCell ref="S28:AC29"/>
-    <mergeCell ref="AE28:AO29"/>
-    <mergeCell ref="S30:Y30"/>
-    <mergeCell ref="AL30:AN30"/>
-    <mergeCell ref="S19:AC19"/>
-    <mergeCell ref="AK19:AN19"/>
-    <mergeCell ref="AK20:AN20"/>
-    <mergeCell ref="AK24:AN24"/>
-    <mergeCell ref="AK25:AN25"/>
-    <mergeCell ref="S20:AC20"/>
-    <mergeCell ref="S22:AH22"/>
-    <mergeCell ref="AK22:AN22"/>
-    <mergeCell ref="S23:AH23"/>
-    <mergeCell ref="AK23:AN23"/>
-    <mergeCell ref="S24:AH24"/>
-    <mergeCell ref="S25:AH25"/>
-    <mergeCell ref="AE19:AH19"/>
-    <mergeCell ref="AE20:AH20"/>
-    <mergeCell ref="S21:AL21"/>
-    <mergeCell ref="AE17:AH17"/>
-    <mergeCell ref="AK17:AN17"/>
-    <mergeCell ref="S17:AC17"/>
-    <mergeCell ref="S18:AC18"/>
-    <mergeCell ref="AE18:AH18"/>
-    <mergeCell ref="AK18:AN18"/>
     <mergeCell ref="AK15:AL15"/>
     <mergeCell ref="AM15:AN15"/>
-    <mergeCell ref="S16:AB16"/>
-    <mergeCell ref="AE16:AH16"/>
-    <mergeCell ref="AK16:AN16"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="H16:L16"/>
   </mergeCells>
   <conditionalFormatting sqref="M16:M17 M19 M25">
     <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="No Match">
@@ -65125,7 +65128,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageSetup scale="53" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>